<commit_message>
Final changes have been made ready to be added in article and presentation.
</commit_message>
<xml_diff>
--- a/Yeni Veri/total_sonuc_keywords.xlsx
+++ b/Yeni Veri/total_sonuc_keywords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bkkas/Documents/TEZ/Tez/Yeni Veri/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B2A60B-B53A-334E-AA4A-0BC10D6E1231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E056C1-BBAF-C94F-8AA6-4ABBF496B67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="635">
   <si>
     <t>StudentID</t>
   </si>
@@ -1936,12 +1936,6 @@
   </si>
   <si>
     <t>DistilBert Score</t>
-  </si>
-  <si>
-    <t>DistilBert Score v2</t>
-  </si>
-  <si>
-    <t>Instructor Score</t>
   </si>
   <si>
     <t>T5 Score</t>
@@ -1963,7 +1957,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -9678,13 +9671,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H134"/>
+  <dimension ref="A1:F134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9703,14 +9696,8 @@
       <c r="F1" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20190808014</v>
       </c>
@@ -9727,16 +9714,10 @@
         <v>57</v>
       </c>
       <c r="F2">
-        <v>35</v>
-      </c>
-      <c r="G2">
-        <v>87</v>
-      </c>
-      <c r="H2">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20190808021</v>
       </c>
@@ -9753,16 +9734,10 @@
         <v>54</v>
       </c>
       <c r="F3">
-        <v>28</v>
-      </c>
-      <c r="G3">
-        <v>85</v>
-      </c>
-      <c r="H3">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20190808035</v>
       </c>
@@ -9779,16 +9754,10 @@
         <v>33</v>
       </c>
       <c r="F4">
-        <v>12</v>
-      </c>
-      <c r="G4">
-        <v>64</v>
-      </c>
-      <c r="H4">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20200808003</v>
       </c>
@@ -9805,16 +9774,10 @@
         <v>25</v>
       </c>
       <c r="F5">
-        <v>25</v>
-      </c>
-      <c r="G5">
-        <v>51</v>
-      </c>
-      <c r="H5">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20200808008</v>
       </c>
@@ -9831,16 +9794,10 @@
         <v>50</v>
       </c>
       <c r="F6">
-        <v>29</v>
-      </c>
-      <c r="G6">
-        <v>84</v>
-      </c>
-      <c r="H6">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20200808015</v>
       </c>
@@ -9857,16 +9814,10 @@
         <v>23</v>
       </c>
       <c r="F7">
-        <v>18</v>
-      </c>
-      <c r="G7">
-        <v>35</v>
-      </c>
-      <c r="H7">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20200808020</v>
       </c>
@@ -9883,16 +9834,10 @@
         <v>41</v>
       </c>
       <c r="F8">
-        <v>29</v>
-      </c>
-      <c r="G8">
-        <v>69</v>
-      </c>
-      <c r="H8">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20200808026</v>
       </c>
@@ -9909,16 +9854,10 @@
         <v>37</v>
       </c>
       <c r="F9">
-        <v>27</v>
-      </c>
-      <c r="G9">
-        <v>67</v>
-      </c>
-      <c r="H9">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20200808033</v>
       </c>
@@ -9935,16 +9874,10 @@
         <v>53</v>
       </c>
       <c r="F10">
-        <v>27</v>
-      </c>
-      <c r="G10">
-        <v>84</v>
-      </c>
-      <c r="H10">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20200808038</v>
       </c>
@@ -9961,16 +9894,10 @@
         <v>50</v>
       </c>
       <c r="F11">
-        <v>31</v>
-      </c>
-      <c r="G11">
-        <v>83</v>
-      </c>
-      <c r="H11">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20200808045</v>
       </c>
@@ -9987,16 +9914,10 @@
         <v>39</v>
       </c>
       <c r="F12">
-        <v>23</v>
-      </c>
-      <c r="G12">
-        <v>68</v>
-      </c>
-      <c r="H12">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20200808062</v>
       </c>
@@ -10013,16 +9934,10 @@
         <v>40</v>
       </c>
       <c r="F13">
-        <v>21</v>
-      </c>
-      <c r="G13">
-        <v>68</v>
-      </c>
-      <c r="H13">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20200808063</v>
       </c>
@@ -10039,16 +9954,10 @@
         <v>21</v>
       </c>
       <c r="F14">
-        <v>6</v>
-      </c>
-      <c r="G14">
-        <v>64</v>
-      </c>
-      <c r="H14">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20200808072</v>
       </c>
@@ -10065,16 +9974,10 @@
         <v>23</v>
       </c>
       <c r="F15">
-        <v>11</v>
-      </c>
-      <c r="G15">
-        <v>51</v>
-      </c>
-      <c r="H15">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20200808504</v>
       </c>
@@ -10091,16 +9994,10 @@
         <v>35</v>
       </c>
       <c r="F16">
-        <v>26</v>
-      </c>
-      <c r="G16">
-        <v>66</v>
-      </c>
-      <c r="H16">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20200808505</v>
       </c>
@@ -10117,16 +10014,10 @@
         <v>26</v>
       </c>
       <c r="F17">
-        <v>17</v>
-      </c>
-      <c r="G17">
-        <v>49</v>
-      </c>
-      <c r="H17">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20200808805</v>
       </c>
@@ -10143,16 +10034,10 @@
         <v>36</v>
       </c>
       <c r="F18">
-        <v>23</v>
-      </c>
-      <c r="G18">
-        <v>68</v>
-      </c>
-      <c r="H18">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20210808005</v>
       </c>
@@ -10169,16 +10054,10 @@
         <v>35</v>
       </c>
       <c r="F19">
-        <v>20</v>
-      </c>
-      <c r="G19">
-        <v>68</v>
-      </c>
-      <c r="H19">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20210808006</v>
       </c>
@@ -10195,16 +10074,10 @@
         <v>37</v>
       </c>
       <c r="F20">
-        <v>30</v>
-      </c>
-      <c r="G20">
-        <v>68</v>
-      </c>
-      <c r="H20">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20210808012</v>
       </c>
@@ -10221,16 +10094,10 @@
         <v>35</v>
       </c>
       <c r="F21">
-        <v>28</v>
-      </c>
-      <c r="G21">
-        <v>67</v>
-      </c>
-      <c r="H21">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20210808014</v>
       </c>
@@ -10247,16 +10114,10 @@
         <v>43</v>
       </c>
       <c r="F22">
-        <v>20</v>
-      </c>
-      <c r="G22">
-        <v>68</v>
-      </c>
-      <c r="H22">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20210808016</v>
       </c>
@@ -10273,16 +10134,10 @@
         <v>17</v>
       </c>
       <c r="F23">
-        <v>6</v>
-      </c>
-      <c r="G23">
-        <v>49</v>
-      </c>
-      <c r="H23">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20210808017</v>
       </c>
@@ -10299,16 +10154,10 @@
         <v>44</v>
       </c>
       <c r="F24">
-        <v>36</v>
-      </c>
-      <c r="G24">
-        <v>69</v>
-      </c>
-      <c r="H24">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20210808018</v>
       </c>
@@ -10325,16 +10174,10 @@
         <v>26</v>
       </c>
       <c r="F25">
-        <v>12</v>
-      </c>
-      <c r="G25">
-        <v>65</v>
-      </c>
-      <c r="H25">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20210808021</v>
       </c>
@@ -10351,16 +10194,10 @@
         <v>20</v>
       </c>
       <c r="F26">
-        <v>18</v>
-      </c>
-      <c r="G26">
-        <v>34</v>
-      </c>
-      <c r="H26">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20210808022</v>
       </c>
@@ -10377,16 +10214,10 @@
         <v>40</v>
       </c>
       <c r="F27">
-        <v>37</v>
-      </c>
-      <c r="G27">
-        <v>69</v>
-      </c>
-      <c r="H27">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20210808025</v>
       </c>
@@ -10403,16 +10234,10 @@
         <v>34</v>
       </c>
       <c r="F28">
-        <v>17</v>
-      </c>
-      <c r="G28">
-        <v>51</v>
-      </c>
-      <c r="H28">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20210808033</v>
       </c>
@@ -10429,16 +10254,10 @@
         <v>29</v>
       </c>
       <c r="F29">
-        <v>25</v>
-      </c>
-      <c r="G29">
-        <v>52</v>
-      </c>
-      <c r="H29">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20210808035</v>
       </c>
@@ -10455,16 +10274,10 @@
         <v>30</v>
       </c>
       <c r="F30">
-        <v>21</v>
-      </c>
-      <c r="G30">
-        <v>66</v>
-      </c>
-      <c r="H30">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20210808038</v>
       </c>
@@ -10481,16 +10294,10 @@
         <v>49</v>
       </c>
       <c r="F31">
-        <v>29</v>
-      </c>
-      <c r="G31">
-        <v>83</v>
-      </c>
-      <c r="H31">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>20210808042</v>
       </c>
@@ -10507,16 +10314,10 @@
         <v>34</v>
       </c>
       <c r="F32">
-        <v>20</v>
-      </c>
-      <c r="G32">
-        <v>67</v>
-      </c>
-      <c r="H32">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20210808044</v>
       </c>
@@ -10533,16 +10334,10 @@
         <v>33</v>
       </c>
       <c r="F33">
-        <v>21</v>
-      </c>
-      <c r="G33">
-        <v>66</v>
-      </c>
-      <c r="H33">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>20210808048</v>
       </c>
@@ -10559,16 +10354,10 @@
         <v>21</v>
       </c>
       <c r="F34">
-        <v>8</v>
-      </c>
-      <c r="G34">
-        <v>34</v>
-      </c>
-      <c r="H34">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>20210808056</v>
       </c>
@@ -10585,16 +10374,10 @@
         <v>32</v>
       </c>
       <c r="F35">
-        <v>24</v>
-      </c>
-      <c r="G35">
-        <v>53</v>
-      </c>
-      <c r="H35">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20210808061</v>
       </c>
@@ -10611,16 +10394,10 @@
         <v>40</v>
       </c>
       <c r="F36">
-        <v>26</v>
-      </c>
-      <c r="G36">
-        <v>68</v>
-      </c>
-      <c r="H36">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>20210808062</v>
       </c>
@@ -10637,16 +10414,10 @@
         <v>35</v>
       </c>
       <c r="F37">
-        <v>27</v>
-      </c>
-      <c r="G37">
-        <v>82</v>
-      </c>
-      <c r="H37">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>20210808065</v>
       </c>
@@ -10663,16 +10434,10 @@
         <v>25</v>
       </c>
       <c r="F38">
-        <v>12</v>
-      </c>
-      <c r="G38">
-        <v>49</v>
-      </c>
-      <c r="H38">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>20210808066</v>
       </c>
@@ -10689,16 +10454,10 @@
         <v>43</v>
       </c>
       <c r="F39">
-        <v>26</v>
-      </c>
-      <c r="G39">
-        <v>82</v>
-      </c>
-      <c r="H39">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>20210808076</v>
       </c>
@@ -10715,16 +10474,10 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>20210808604</v>
       </c>
@@ -10741,16 +10494,10 @@
         <v>37</v>
       </c>
       <c r="F41">
-        <v>25</v>
-      </c>
-      <c r="G41">
-        <v>66</v>
-      </c>
-      <c r="H41">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>20210808605</v>
       </c>
@@ -10767,16 +10514,10 @@
         <v>42</v>
       </c>
       <c r="F42">
-        <v>26</v>
-      </c>
-      <c r="G42">
-        <v>68</v>
-      </c>
-      <c r="H42">
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>20210808608</v>
       </c>
@@ -10793,16 +10534,10 @@
         <v>23</v>
       </c>
       <c r="F43">
-        <v>18</v>
-      </c>
-      <c r="G43">
-        <v>34</v>
-      </c>
-      <c r="H43">
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>20210808610</v>
       </c>
@@ -10819,16 +10554,10 @@
         <v>9</v>
       </c>
       <c r="F44">
-        <v>4</v>
-      </c>
-      <c r="G44">
-        <v>33</v>
-      </c>
-      <c r="H44">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>20210808612</v>
       </c>
@@ -10845,16 +10574,10 @@
         <v>34</v>
       </c>
       <c r="F45">
-        <v>25</v>
-      </c>
-      <c r="G45">
-        <v>67</v>
-      </c>
-      <c r="H45">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>20210808614</v>
       </c>
@@ -10871,16 +10594,10 @@
         <v>30</v>
       </c>
       <c r="F46">
-        <v>19</v>
-      </c>
-      <c r="G46">
-        <v>51</v>
-      </c>
-      <c r="H46">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>20210808615</v>
       </c>
@@ -10897,16 +10614,10 @@
         <v>41</v>
       </c>
       <c r="F47">
-        <v>28</v>
-      </c>
-      <c r="G47">
-        <v>68</v>
-      </c>
-      <c r="H47">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>20210808616</v>
       </c>
@@ -10923,16 +10634,10 @@
         <v>32</v>
       </c>
       <c r="F48">
-        <v>18</v>
-      </c>
-      <c r="G48">
-        <v>52</v>
-      </c>
-      <c r="H48">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>20220808001</v>
       </c>
@@ -10949,16 +10654,10 @@
         <v>38</v>
       </c>
       <c r="F49">
-        <v>30</v>
-      </c>
-      <c r="G49">
-        <v>68</v>
-      </c>
-      <c r="H49">
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>20220808002</v>
       </c>
@@ -10975,16 +10674,10 @@
         <v>37</v>
       </c>
       <c r="F50">
-        <v>16</v>
-      </c>
-      <c r="G50">
-        <v>64</v>
-      </c>
-      <c r="H50">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>20220808005</v>
       </c>
@@ -11001,16 +10694,10 @@
         <v>51</v>
       </c>
       <c r="F51">
-        <v>26</v>
-      </c>
-      <c r="G51">
-        <v>83</v>
-      </c>
-      <c r="H51">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>20220808006</v>
       </c>
@@ -11027,16 +10714,10 @@
         <v>55</v>
       </c>
       <c r="F52">
-        <v>31</v>
-      </c>
-      <c r="G52">
-        <v>85</v>
-      </c>
-      <c r="H52">
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>20220808007</v>
       </c>
@@ -11053,16 +10734,10 @@
         <v>30</v>
       </c>
       <c r="F53">
-        <v>22</v>
-      </c>
-      <c r="G53">
-        <v>51</v>
-      </c>
-      <c r="H53">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>20220808010</v>
       </c>
@@ -11079,16 +10754,10 @@
         <v>24</v>
       </c>
       <c r="F54">
-        <v>13</v>
-      </c>
-      <c r="G54">
-        <v>50</v>
-      </c>
-      <c r="H54">
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>20220808013</v>
       </c>
@@ -11105,16 +10774,10 @@
         <v>35</v>
       </c>
       <c r="F55">
-        <v>20</v>
-      </c>
-      <c r="G55">
-        <v>66</v>
-      </c>
-      <c r="H55">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>20220808014</v>
       </c>
@@ -11131,16 +10794,10 @@
         <v>26</v>
       </c>
       <c r="F56">
-        <v>19</v>
-      </c>
-      <c r="G56">
-        <v>50</v>
-      </c>
-      <c r="H56">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>20220808016</v>
       </c>
@@ -11157,16 +10814,10 @@
         <v>25</v>
       </c>
       <c r="F57">
-        <v>21</v>
-      </c>
-      <c r="G57">
-        <v>50</v>
-      </c>
-      <c r="H57">
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>20220808018</v>
       </c>
@@ -11183,16 +10834,10 @@
         <v>35</v>
       </c>
       <c r="F58">
-        <v>23</v>
-      </c>
-      <c r="G58">
-        <v>68</v>
-      </c>
-      <c r="H58">
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>20220808019</v>
       </c>
@@ -11209,16 +10854,10 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>0</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>20220808022</v>
       </c>
@@ -11235,16 +10874,10 @@
         <v>26</v>
       </c>
       <c r="F60">
-        <v>16</v>
-      </c>
-      <c r="G60">
-        <v>51</v>
-      </c>
-      <c r="H60">
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>20220808023</v>
       </c>
@@ -11261,16 +10894,10 @@
         <v>54</v>
       </c>
       <c r="F61">
-        <v>33</v>
-      </c>
-      <c r="G61">
-        <v>84</v>
-      </c>
-      <c r="H61">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>20220808024</v>
       </c>
@@ -11287,16 +10914,10 @@
         <v>39</v>
       </c>
       <c r="F62">
-        <v>22</v>
-      </c>
-      <c r="G62">
-        <v>66</v>
-      </c>
-      <c r="H62">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>20220808025</v>
       </c>
@@ -11313,16 +10934,10 @@
         <v>40</v>
       </c>
       <c r="F63">
-        <v>31</v>
-      </c>
-      <c r="G63">
-        <v>68</v>
-      </c>
-      <c r="H63">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>20220808026</v>
       </c>
@@ -11339,16 +10954,10 @@
         <v>10</v>
       </c>
       <c r="F64">
-        <v>6</v>
-      </c>
-      <c r="G64">
-        <v>16</v>
-      </c>
-      <c r="H64">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>20220808028</v>
       </c>
@@ -11365,16 +10974,10 @@
         <v>39</v>
       </c>
       <c r="F65">
-        <v>30</v>
-      </c>
-      <c r="G65">
-        <v>82</v>
-      </c>
-      <c r="H65">
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>20220808029</v>
       </c>
@@ -11391,16 +10994,10 @@
         <v>27</v>
       </c>
       <c r="F66">
-        <v>21</v>
-      </c>
-      <c r="G66">
-        <v>51</v>
-      </c>
-      <c r="H66">
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>20220808032</v>
       </c>
@@ -11417,16 +11014,10 @@
         <v>36</v>
       </c>
       <c r="F67">
-        <v>34</v>
-      </c>
-      <c r="G67">
-        <v>69</v>
-      </c>
-      <c r="H67">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>20220808033</v>
       </c>
@@ -11443,16 +11034,10 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>20220808034</v>
       </c>
@@ -11469,16 +11054,10 @@
         <v>24</v>
       </c>
       <c r="F69">
-        <v>14</v>
-      </c>
-      <c r="G69">
-        <v>35</v>
-      </c>
-      <c r="H69">
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>20220808035</v>
       </c>
@@ -11495,16 +11074,10 @@
         <v>24</v>
       </c>
       <c r="F70">
-        <v>24</v>
-      </c>
-      <c r="G70">
-        <v>36</v>
-      </c>
-      <c r="H70">
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>20220808037</v>
       </c>
@@ -11521,16 +11094,10 @@
         <v>45</v>
       </c>
       <c r="F71">
-        <v>28</v>
-      </c>
-      <c r="G71">
-        <v>83</v>
-      </c>
-      <c r="H71">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>20220808038</v>
       </c>
@@ -11547,16 +11114,10 @@
         <v>50</v>
       </c>
       <c r="F72">
-        <v>40</v>
-      </c>
-      <c r="G72">
-        <v>85</v>
-      </c>
-      <c r="H72">
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>20220808039</v>
       </c>
@@ -11573,16 +11134,10 @@
         <v>38</v>
       </c>
       <c r="F73">
-        <v>24</v>
-      </c>
-      <c r="G73">
-        <v>66</v>
-      </c>
-      <c r="H73">
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>20220808041</v>
       </c>
@@ -11599,16 +11154,10 @@
         <v>46</v>
       </c>
       <c r="F74">
-        <v>28</v>
-      </c>
-      <c r="G74">
-        <v>85</v>
-      </c>
-      <c r="H74">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>20220808043</v>
       </c>
@@ -11625,16 +11174,10 @@
         <v>34</v>
       </c>
       <c r="F75">
-        <v>17</v>
-      </c>
-      <c r="G75">
-        <v>51</v>
-      </c>
-      <c r="H75">
         <v>48</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>20220808044</v>
       </c>
@@ -11651,16 +11194,10 @@
         <v>49</v>
       </c>
       <c r="F76">
-        <v>30</v>
-      </c>
-      <c r="G76">
-        <v>85</v>
-      </c>
-      <c r="H76">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>20220808045</v>
       </c>
@@ -11677,16 +11214,10 @@
         <v>26</v>
       </c>
       <c r="F77">
-        <v>7</v>
-      </c>
-      <c r="G77">
-        <v>50</v>
-      </c>
-      <c r="H77">
         <v>43</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>20220808046</v>
       </c>
@@ -11703,16 +11234,10 @@
         <v>17</v>
       </c>
       <c r="F78">
-        <v>12</v>
-      </c>
-      <c r="G78">
-        <v>32</v>
-      </c>
-      <c r="H78">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>20220808047</v>
       </c>
@@ -11729,16 +11254,10 @@
         <v>34</v>
       </c>
       <c r="F79">
-        <v>8</v>
-      </c>
-      <c r="G79">
-        <v>65</v>
-      </c>
-      <c r="H79">
         <v>54</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>20220808048</v>
       </c>
@@ -11755,16 +11274,10 @@
         <v>49</v>
       </c>
       <c r="F80">
-        <v>26</v>
-      </c>
-      <c r="G80">
-        <v>85</v>
-      </c>
-      <c r="H80">
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>20220808050</v>
       </c>
@@ -11781,16 +11294,10 @@
         <v>0</v>
       </c>
       <c r="F81">
-        <v>0</v>
-      </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-      <c r="H81">
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>20220808051</v>
       </c>
@@ -11807,16 +11314,10 @@
         <v>27</v>
       </c>
       <c r="F82">
-        <v>20</v>
-      </c>
-      <c r="G82">
-        <v>51</v>
-      </c>
-      <c r="H82">
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>20220808052</v>
       </c>
@@ -11833,16 +11334,10 @@
         <v>39</v>
       </c>
       <c r="F83">
-        <v>31</v>
-      </c>
-      <c r="G83">
-        <v>67</v>
-      </c>
-      <c r="H83">
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>20220808053</v>
       </c>
@@ -11859,16 +11354,10 @@
         <v>49</v>
       </c>
       <c r="F84">
-        <v>37</v>
-      </c>
-      <c r="G84">
-        <v>85</v>
-      </c>
-      <c r="H84">
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>20220808055</v>
       </c>
@@ -11885,16 +11374,10 @@
         <v>52</v>
       </c>
       <c r="F85">
-        <v>30</v>
-      </c>
-      <c r="G85">
-        <v>84</v>
-      </c>
-      <c r="H85">
         <v>74</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>20220808056</v>
       </c>
@@ -11911,16 +11394,10 @@
         <v>40</v>
       </c>
       <c r="F86">
-        <v>29</v>
-      </c>
-      <c r="G86">
-        <v>69</v>
-      </c>
-      <c r="H86">
         <v>61</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>20220808057</v>
       </c>
@@ -11937,16 +11414,10 @@
         <v>49</v>
       </c>
       <c r="F87">
-        <v>29</v>
-      </c>
-      <c r="G87">
-        <v>85</v>
-      </c>
-      <c r="H87">
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>20220808058</v>
       </c>
@@ -11963,16 +11434,10 @@
         <v>51</v>
       </c>
       <c r="F88">
-        <v>35</v>
-      </c>
-      <c r="G88">
-        <v>83</v>
-      </c>
-      <c r="H88">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>20220808059</v>
       </c>
@@ -11989,16 +11454,10 @@
         <v>37</v>
       </c>
       <c r="F89">
-        <v>21</v>
-      </c>
-      <c r="G89">
-        <v>68</v>
-      </c>
-      <c r="H89">
         <v>61</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>20220808060</v>
       </c>
@@ -12015,16 +11474,10 @@
         <v>27</v>
       </c>
       <c r="F90">
-        <v>20</v>
-      </c>
-      <c r="G90">
-        <v>37</v>
-      </c>
-      <c r="H90">
         <v>34</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>20220808062</v>
       </c>
@@ -12041,16 +11494,10 @@
         <v>38</v>
       </c>
       <c r="F91">
-        <v>16</v>
-      </c>
-      <c r="G91">
-        <v>65</v>
-      </c>
-      <c r="H91">
         <v>55</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>20220808063</v>
       </c>
@@ -12067,16 +11514,10 @@
         <v>29</v>
       </c>
       <c r="F92">
-        <v>22</v>
-      </c>
-      <c r="G92">
-        <v>66</v>
-      </c>
-      <c r="H92">
         <v>55</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>20220808066</v>
       </c>
@@ -12093,16 +11534,10 @@
         <v>20</v>
       </c>
       <c r="F93">
-        <v>13</v>
-      </c>
-      <c r="G93">
-        <v>50</v>
-      </c>
-      <c r="H93">
         <v>44</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>20220808067</v>
       </c>
@@ -12119,16 +11554,10 @@
         <v>38</v>
       </c>
       <c r="F94">
-        <v>29</v>
-      </c>
-      <c r="G94">
-        <v>66</v>
-      </c>
-      <c r="H94">
         <v>58</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>20220808069</v>
       </c>
@@ -12145,16 +11574,10 @@
         <v>47</v>
       </c>
       <c r="F95">
-        <v>30</v>
-      </c>
-      <c r="G95">
-        <v>83</v>
-      </c>
-      <c r="H95">
         <v>72</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>20220808071</v>
       </c>
@@ -12171,16 +11594,10 @@
         <v>23</v>
       </c>
       <c r="F96">
-        <v>19</v>
-      </c>
-      <c r="G96">
-        <v>49</v>
-      </c>
-      <c r="H96">
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>20220808072</v>
       </c>
@@ -12197,16 +11614,10 @@
         <v>38</v>
       </c>
       <c r="F97">
-        <v>20</v>
-      </c>
-      <c r="G97">
-        <v>66</v>
-      </c>
-      <c r="H97">
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>20220808073</v>
       </c>
@@ -12223,16 +11634,10 @@
         <v>41</v>
       </c>
       <c r="F98">
-        <v>27</v>
-      </c>
-      <c r="G98">
-        <v>68</v>
-      </c>
-      <c r="H98">
         <v>60</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>20220808074</v>
       </c>
@@ -12249,16 +11654,10 @@
         <v>38</v>
       </c>
       <c r="F99">
-        <v>26</v>
-      </c>
-      <c r="G99">
-        <v>67</v>
-      </c>
-      <c r="H99">
         <v>58</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>20220808076</v>
       </c>
@@ -12275,16 +11674,10 @@
         <v>19</v>
       </c>
       <c r="F100">
-        <v>6</v>
-      </c>
-      <c r="G100">
-        <v>33</v>
-      </c>
-      <c r="H100">
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>20220808077</v>
       </c>
@@ -12301,16 +11694,10 @@
         <v>39</v>
       </c>
       <c r="F101">
-        <v>32</v>
-      </c>
-      <c r="G101">
-        <v>82</v>
-      </c>
-      <c r="H101">
         <v>70</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>20220808504</v>
       </c>
@@ -12327,16 +11714,10 @@
         <v>38</v>
       </c>
       <c r="F102">
-        <v>26</v>
-      </c>
-      <c r="G102">
-        <v>69</v>
-      </c>
-      <c r="H102">
         <v>61</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>20220808601</v>
       </c>
@@ -12353,16 +11734,10 @@
         <v>0</v>
       </c>
       <c r="F103">
-        <v>0</v>
-      </c>
-      <c r="G103">
-        <v>0</v>
-      </c>
-      <c r="H103">
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>20220808604</v>
       </c>
@@ -12379,16 +11754,10 @@
         <v>28</v>
       </c>
       <c r="F104">
-        <v>23</v>
-      </c>
-      <c r="G104">
-        <v>52</v>
-      </c>
-      <c r="H104">
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>20220808606</v>
       </c>
@@ -12405,16 +11774,10 @@
         <v>20</v>
       </c>
       <c r="F105">
-        <v>20</v>
-      </c>
-      <c r="G105">
-        <v>35</v>
-      </c>
-      <c r="H105">
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>20220808607</v>
       </c>
@@ -12431,16 +11794,10 @@
         <v>42</v>
       </c>
       <c r="F106">
-        <v>18</v>
-      </c>
-      <c r="G106">
-        <v>66</v>
-      </c>
-      <c r="H106">
         <v>58</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>20220808608</v>
       </c>
@@ -12457,16 +11814,10 @@
         <v>26</v>
       </c>
       <c r="F107">
-        <v>18</v>
-      </c>
-      <c r="G107">
-        <v>50</v>
-      </c>
-      <c r="H107">
         <v>42</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>20220808610</v>
       </c>
@@ -12483,16 +11834,10 @@
         <v>34</v>
       </c>
       <c r="F108">
-        <v>23</v>
-      </c>
-      <c r="G108">
-        <v>66</v>
-      </c>
-      <c r="H108">
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>20220808616</v>
       </c>
@@ -12509,16 +11854,10 @@
         <v>39</v>
       </c>
       <c r="F109">
-        <v>26</v>
-      </c>
-      <c r="G109">
-        <v>67</v>
-      </c>
-      <c r="H109">
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>20220808617</v>
       </c>
@@ -12535,16 +11874,10 @@
         <v>40</v>
       </c>
       <c r="F110">
-        <v>29</v>
-      </c>
-      <c r="G110">
-        <v>67</v>
-      </c>
-      <c r="H110">
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>20220808703</v>
       </c>
@@ -12561,16 +11894,10 @@
         <v>36</v>
       </c>
       <c r="F111">
-        <v>22</v>
-      </c>
-      <c r="G111">
-        <v>68</v>
-      </c>
-      <c r="H111">
         <v>60</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>20220808705</v>
       </c>
@@ -12587,16 +11914,10 @@
         <v>29</v>
       </c>
       <c r="F112">
-        <v>23</v>
-      </c>
-      <c r="G112">
-        <v>52</v>
-      </c>
-      <c r="H112">
         <v>45</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>20220808706</v>
       </c>
@@ -12613,16 +11934,10 @@
         <v>19</v>
       </c>
       <c r="F113">
-        <v>17</v>
-      </c>
-      <c r="G113">
-        <v>64</v>
-      </c>
-      <c r="H113">
         <v>53</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>20230808004</v>
       </c>
@@ -12639,16 +11954,10 @@
         <v>39</v>
       </c>
       <c r="F114">
-        <v>32</v>
-      </c>
-      <c r="G114">
-        <v>69</v>
-      </c>
-      <c r="H114">
         <v>61</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>20230808010</v>
       </c>
@@ -12665,16 +11974,10 @@
         <v>48</v>
       </c>
       <c r="F115">
-        <v>35</v>
-      </c>
-      <c r="G115">
-        <v>86</v>
-      </c>
-      <c r="H115">
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>20230808020</v>
       </c>
@@ -12691,16 +11994,10 @@
         <v>16</v>
       </c>
       <c r="F116">
-        <v>11</v>
-      </c>
-      <c r="G116">
-        <v>48</v>
-      </c>
-      <c r="H116">
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>20230808049</v>
       </c>
@@ -12717,16 +12014,10 @@
         <v>53</v>
       </c>
       <c r="F117">
-        <v>33</v>
-      </c>
-      <c r="G117">
-        <v>85</v>
-      </c>
-      <c r="H117">
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>20230808055</v>
       </c>
@@ -12743,16 +12034,10 @@
         <v>38</v>
       </c>
       <c r="F118">
-        <v>29</v>
-      </c>
-      <c r="G118">
-        <v>66</v>
-      </c>
-      <c r="H118">
         <v>56</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>20230808061</v>
       </c>
@@ -12769,16 +12054,10 @@
         <v>44</v>
       </c>
       <c r="F119">
-        <v>29</v>
-      </c>
-      <c r="G119">
-        <v>81</v>
-      </c>
-      <c r="H119">
         <v>70</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>20230808062</v>
       </c>
@@ -12795,16 +12074,10 @@
         <v>49</v>
       </c>
       <c r="F120">
-        <v>26</v>
-      </c>
-      <c r="G120">
-        <v>84</v>
-      </c>
-      <c r="H120">
         <v>72</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>20230808066</v>
       </c>
@@ -12821,16 +12094,10 @@
         <v>42</v>
       </c>
       <c r="F121">
-        <v>24</v>
-      </c>
-      <c r="G121">
-        <v>69</v>
-      </c>
-      <c r="H121">
         <v>61</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>20230808070</v>
       </c>
@@ -12847,16 +12114,10 @@
         <v>30</v>
       </c>
       <c r="F122">
-        <v>18</v>
-      </c>
-      <c r="G122">
-        <v>50</v>
-      </c>
-      <c r="H122">
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>20230808075</v>
       </c>
@@ -12873,16 +12134,10 @@
         <v>49</v>
       </c>
       <c r="F123">
-        <v>34</v>
-      </c>
-      <c r="G123">
-        <v>84</v>
-      </c>
-      <c r="H123">
         <v>74</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>20230808077</v>
       </c>
@@ -12899,16 +12154,10 @@
         <v>32</v>
       </c>
       <c r="F124">
-        <v>25</v>
-      </c>
-      <c r="G124">
-        <v>51</v>
-      </c>
-      <c r="H124">
         <v>48</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>20230808602</v>
       </c>
@@ -12925,16 +12174,10 @@
         <v>0</v>
       </c>
       <c r="F125">
-        <v>0</v>
-      </c>
-      <c r="G125">
-        <v>0</v>
-      </c>
-      <c r="H125">
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>20230808608</v>
       </c>
@@ -12951,16 +12194,10 @@
         <v>29</v>
       </c>
       <c r="F126">
-        <v>21</v>
-      </c>
-      <c r="G126">
-        <v>53</v>
-      </c>
-      <c r="H126">
         <v>48</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>20230808609</v>
       </c>
@@ -12977,16 +12214,10 @@
         <v>23</v>
       </c>
       <c r="F127">
-        <v>27</v>
-      </c>
-      <c r="G127">
-        <v>49</v>
-      </c>
-      <c r="H127">
         <v>40</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>20230808611</v>
       </c>
@@ -13003,16 +12234,10 @@
         <v>34</v>
       </c>
       <c r="F128">
-        <v>21</v>
-      </c>
-      <c r="G128">
-        <v>69</v>
-      </c>
-      <c r="H128">
         <v>61</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>20230808614</v>
       </c>
@@ -13029,16 +12254,10 @@
         <v>47</v>
       </c>
       <c r="F129">
-        <v>30</v>
-      </c>
-      <c r="G129">
-        <v>84</v>
-      </c>
-      <c r="H129">
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>20230808615</v>
       </c>
@@ -13055,16 +12274,10 @@
         <v>40</v>
       </c>
       <c r="F130">
-        <v>23</v>
-      </c>
-      <c r="G130">
-        <v>82</v>
-      </c>
-      <c r="H130">
         <v>70</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>20230808617</v>
       </c>
@@ -13081,16 +12294,10 @@
         <v>40</v>
       </c>
       <c r="F131">
-        <v>18</v>
-      </c>
-      <c r="G131">
-        <v>67</v>
-      </c>
-      <c r="H131">
         <v>58</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>20230808618</v>
       </c>
@@ -13107,16 +12314,10 @@
         <v>35</v>
       </c>
       <c r="F132">
-        <v>20</v>
-      </c>
-      <c r="G132">
-        <v>66</v>
-      </c>
-      <c r="H132">
         <v>54</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>20230808621</v>
       </c>
@@ -13133,16 +12334,10 @@
         <v>46</v>
       </c>
       <c r="F133">
-        <v>32</v>
-      </c>
-      <c r="G133">
-        <v>68</v>
-      </c>
-      <c r="H133">
         <v>61</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>20230808623</v>
       </c>
@@ -13159,12 +12354,6 @@
         <v>51</v>
       </c>
       <c r="F134">
-        <v>31</v>
-      </c>
-      <c r="G134">
-        <v>83</v>
-      </c>
-      <c r="H134">
         <v>75</v>
       </c>
     </row>

</xml_diff>